<commit_message>
ispunjen 11. zahtev i ulepsan ostatak koda
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sj_ruby_domacizadatak\sj_ruby_domacizadatak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0798B7F-E6E0-48EC-B2E9-CDD76E22721F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E97F19B-5834-4997-B70B-9C115DA13D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,11 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,7 +383,7 @@
   <dimension ref="E23:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G26"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,22 +403,16 @@
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <v>9</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>6</v>
-      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
         <v>5</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="2">
+        <v>6</v>
+      </c>
       <c r="H25">
         <v>8</v>
       </c>
@@ -426,7 +421,9 @@
       <c r="F26">
         <v>2</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E27">
@@ -442,17 +439,16 @@
     <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E28">
         <f>SUBTOTAL(9, E24:E27)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G28">
         <f>SUBTOTAL(9,G24:G27)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G24:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>